<commit_message>
controle da presença (dia 19/09/2022) e  notas do fórum para a semana 11/09/2022 a 17/09/2022
</commit_message>
<xml_diff>
--- a/build/ensino/2022/08/segundo-semestre-de-2022/mes-8-dia-21-ava-matc65.xlsx
+++ b/build/ensino/2022/08/segundo-semestre-de-2022/mes-8-dia-21-ava-matc65.xlsx
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -566,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -598,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -630,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="J8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -694,7 +694,7 @@
         <v>3</v>
       </c>
       <c r="J10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -726,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -790,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="J14">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -854,7 +854,7 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -918,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="J17">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -982,7 +982,7 @@
         <v>2</v>
       </c>
       <c r="J19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -1014,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="J21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="J22">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
@@ -1110,7 +1110,7 @@
         <v>3</v>
       </c>
       <c r="J23">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -1142,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="J24">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1174,7 +1174,7 @@
         <v>2</v>
       </c>
       <c r="J25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1206,7 +1206,7 @@
         <v>4</v>
       </c>
       <c r="J26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1270,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="J28">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1302,7 +1302,7 @@
         <v>2</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -1334,7 +1334,7 @@
         <v>2</v>
       </c>
       <c r="J30">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1398,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1462,7 +1462,7 @@
         <v>2</v>
       </c>
       <c r="J34">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -1494,7 +1494,7 @@
         <v>2</v>
       </c>
       <c r="J35">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1526,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="J36">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -1590,7 +1590,7 @@
         <v>3</v>
       </c>
       <c r="J38">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1622,7 +1622,7 @@
         <v>3</v>
       </c>
       <c r="J39">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
@@ -1654,7 +1654,7 @@
         <v>2</v>
       </c>
       <c r="J40">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -1686,7 +1686,7 @@
         <v>2</v>
       </c>
       <c r="J41">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
@@ -1718,7 +1718,7 @@
         <v>4</v>
       </c>
       <c r="J42">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -1750,7 +1750,7 @@
         <v>5</v>
       </c>
       <c r="J43">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -1878,7 +1878,7 @@
         <v>4</v>
       </c>
       <c r="J47">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -1942,7 +1942,7 @@
         <v>4</v>
       </c>
       <c r="J49">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -1974,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="J50">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>